<commit_message>
Pva, file names v2.0
+- Pva
+- File names
</commit_message>
<xml_diff>
--- a/documentatie/vergaderingen/agenda_vergadering1.xlsx
+++ b/documentatie/vergaderingen/agenda_vergadering1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\meetings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Youssef\Documents\GitKraken\Barroc-IT-Groep-2\documentatie\vergaderingen\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -187,9 +187,6 @@
     <t>Welkom, vaststellen voorzitter + notulist , vaststellen definitieve agenda</t>
   </si>
   <si>
-    <t xml:space="preserve"> AGENDA Barroc-IT Groep</t>
-  </si>
-  <si>
     <t>Vaststellen volgende vergadering</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>Fedde van Gils</t>
   </si>
   <si>
-    <t>Datum:11 sep 2017</t>
-  </si>
-  <si>
     <t>Locatie: Lokaal BN0329</t>
   </si>
   <si>
@@ -218,6 +212,12 @@
   </si>
   <si>
     <t>Tijd: 10:45</t>
+  </si>
+  <si>
+    <t>Datum: 11 sep 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> AGENDA Barroc-IT Groep 2</t>
   </si>
 </sst>
 </file>
@@ -598,6 +598,17 @@
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="20" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -631,17 +642,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -953,7 +953,7 @@
   <dimension ref="A1:L60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="E3" sqref="E3:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,51 +973,51 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="B3" s="62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="63"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="67"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="66"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="61"/>
+      <c r="B4" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="75"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="70"/>
       <c r="I4" s="5"/>
     </row>
     <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="64"/>
+      <c r="B5" s="77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1059,7 +1059,7 @@
       <c r="E8" s="15">
         <v>1</v>
       </c>
-      <c r="F8" s="73" t="s">
+      <c r="F8" s="52" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="17"/>
@@ -1078,7 +1078,7 @@
       <c r="E9" s="15">
         <v>2</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="57" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="18"/>
@@ -1093,8 +1093,8 @@
       <c r="E10" s="15">
         <v>3</v>
       </c>
-      <c r="F10" s="78" t="s">
-        <v>21</v>
+      <c r="F10" s="57" t="s">
+        <v>20</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
@@ -1109,8 +1109,8 @@
       <c r="E11" s="15">
         <v>4</v>
       </c>
-      <c r="F11" s="79" t="s">
-        <v>25</v>
+      <c r="F11" s="58" t="s">
+        <v>23</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="24"/>
@@ -1125,8 +1125,8 @@
       <c r="E12" s="15">
         <v>5</v>
       </c>
-      <c r="F12" s="71" t="s">
-        <v>26</v>
+      <c r="F12" s="50" t="s">
+        <v>24</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="24"/>
@@ -1141,8 +1141,8 @@
       <c r="E13" s="15">
         <v>6</v>
       </c>
-      <c r="F13" s="75" t="s">
-        <v>27</v>
+      <c r="F13" s="54" t="s">
+        <v>25</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="24"/>
@@ -1157,8 +1157,8 @@
       <c r="E14" s="15">
         <v>7</v>
       </c>
-      <c r="F14" s="75" t="s">
-        <v>28</v>
+      <c r="F14" s="54" t="s">
+        <v>26</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="24"/>
@@ -1175,8 +1175,8 @@
       <c r="E15" s="15">
         <v>8</v>
       </c>
-      <c r="F15" s="74" t="s">
-        <v>20</v>
+      <c r="F15" s="53" t="s">
+        <v>19</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="18"/>
@@ -1193,7 +1193,7 @@
       <c r="E16" s="15">
         <v>9</v>
       </c>
-      <c r="F16" s="72" t="s">
+      <c r="F16" s="51" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="17"/>
@@ -1215,7 +1215,7 @@
         <f>SUM(C8:C17)</f>
         <v>78</v>
       </c>
-      <c r="D18" s="76" t="s">
+      <c r="D18" s="55" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="32" t="s">
@@ -1224,7 +1224,7 @@
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
       <c r="H18" s="34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
       <c r="E26" s="4">
         <v>2</v>
       </c>
-      <c r="F26" s="77"/>
+      <c r="F26" s="56"/>
       <c r="I26" s="47"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1305,7 +1305,7 @@
       <c r="E27" s="4">
         <v>3</v>
       </c>
-      <c r="F27" s="77"/>
+      <c r="F27" s="56"/>
       <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
       <c r="E28" s="4">
         <v>4</v>
       </c>
-      <c r="F28" s="77"/>
+      <c r="F28" s="56"/>
       <c r="G28" s="48"/>
       <c r="H28" s="48"/>
       <c r="I28" s="49"/>
@@ -1493,18 +1493,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1557,14 +1557,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EC78C7E-41AD-4518-BFAA-0ABA4B09AB48}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -1574,6 +1566,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D4A539-5E71-46A4-A076-A8448D6640BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>